<commit_message>
found rgb values for the darker gray trays
</commit_message>
<xml_diff>
--- a/frame_rgbvalues.xlsx
+++ b/frame_rgbvalues.xlsx
@@ -12,13 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="9612" windowHeight="9744"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="frame3" sheetId="1" r:id="rId1"/>
+    <sheet name="frame14(dark)" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$15:$A$41</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$15:$A$41</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$15:$A$41</definedName>
-  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>R</t>
   </si>
@@ -398,7 +394,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -894,4 +890,399 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C34" sqref="A34:C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>97</v>
+      </c>
+      <c r="B2">
+        <v>87</v>
+      </c>
+      <c r="C2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>115</v>
+      </c>
+      <c r="B3">
+        <v>101</v>
+      </c>
+      <c r="C3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>119</v>
+      </c>
+      <c r="B4">
+        <v>102</v>
+      </c>
+      <c r="C4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>126</v>
+      </c>
+      <c r="B5">
+        <v>103</v>
+      </c>
+      <c r="C5">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>196</v>
+      </c>
+      <c r="B6">
+        <v>175</v>
+      </c>
+      <c r="C6">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>159</v>
+      </c>
+      <c r="B7">
+        <v>131</v>
+      </c>
+      <c r="C7">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>190</v>
+      </c>
+      <c r="B8">
+        <v>157</v>
+      </c>
+      <c r="C8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>191</v>
+      </c>
+      <c r="B9">
+        <v>168</v>
+      </c>
+      <c r="C9">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>223</v>
+      </c>
+      <c r="B10">
+        <v>196</v>
+      </c>
+      <c r="C10">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>184</v>
+      </c>
+      <c r="B11">
+        <v>159</v>
+      </c>
+      <c r="C11">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>133</v>
+      </c>
+      <c r="B12">
+        <v>107</v>
+      </c>
+      <c r="C12">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>111</v>
+      </c>
+      <c r="B13">
+        <v>92</v>
+      </c>
+      <c r="C13">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>127</v>
+      </c>
+      <c r="B14">
+        <v>110</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>112</v>
+      </c>
+      <c r="B15">
+        <v>97</v>
+      </c>
+      <c r="C15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>100</v>
+      </c>
+      <c r="B16">
+        <v>93</v>
+      </c>
+      <c r="C16">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>89</v>
+      </c>
+      <c r="B17">
+        <v>83</v>
+      </c>
+      <c r="C17">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>93</v>
+      </c>
+      <c r="B18">
+        <v>82</v>
+      </c>
+      <c r="C18">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>99</v>
+      </c>
+      <c r="B19">
+        <v>89</v>
+      </c>
+      <c r="C19">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>98</v>
+      </c>
+      <c r="B20">
+        <v>86</v>
+      </c>
+      <c r="C20">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>114</v>
+      </c>
+      <c r="B21">
+        <v>95</v>
+      </c>
+      <c r="C21">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>126</v>
+      </c>
+      <c r="B22">
+        <v>106</v>
+      </c>
+      <c r="C22">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>91</v>
+      </c>
+      <c r="B23">
+        <v>92</v>
+      </c>
+      <c r="C23">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>121</v>
+      </c>
+      <c r="B24">
+        <v>115</v>
+      </c>
+      <c r="C24">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>103</v>
+      </c>
+      <c r="B25">
+        <v>100</v>
+      </c>
+      <c r="C25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>133</v>
+      </c>
+      <c r="B26">
+        <v>115</v>
+      </c>
+      <c r="C26">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>122</v>
+      </c>
+      <c r="B27">
+        <v>108</v>
+      </c>
+      <c r="C27">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>123</v>
+      </c>
+      <c r="B28">
+        <v>105</v>
+      </c>
+      <c r="C28">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>209</v>
+      </c>
+      <c r="B29">
+        <v>182</v>
+      </c>
+      <c r="C29">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>177</v>
+      </c>
+      <c r="B30">
+        <v>148</v>
+      </c>
+      <c r="C30">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>114</v>
+      </c>
+      <c r="B31">
+        <v>100</v>
+      </c>
+      <c r="C31">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>124</v>
+      </c>
+      <c r="B32">
+        <v>111</v>
+      </c>
+      <c r="C32">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>110</v>
+      </c>
+      <c r="B33">
+        <v>104</v>
+      </c>
+      <c r="C33">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" ref="A34:B34" si="0">MIN(A2:A33)</f>
+        <v>89</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="C34">
+        <f>MIN(C2:C33)</f>
+        <v>75</v>
+      </c>
+      <c r="D34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added sheet for rgb values of the white tags
</commit_message>
<xml_diff>
--- a/frame_rgbvalues.xlsx
+++ b/frame_rgbvalues.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9612" windowHeight="9744"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9612" windowHeight="9744" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="frame3" sheetId="1" r:id="rId1"/>
     <sheet name="frame14(dark)" sheetId="2" r:id="rId2"/>
+    <sheet name="white tags" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>R</t>
   </si>
@@ -40,6 +41,12 @@
   </si>
   <si>
     <t>minimum</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
@@ -393,7 +400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
@@ -1285,4 +1292,427 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:C36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>255</v>
+      </c>
+      <c r="B2">
+        <v>255</v>
+      </c>
+      <c r="C2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>247</v>
+      </c>
+      <c r="B3">
+        <v>247</v>
+      </c>
+      <c r="C3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>252</v>
+      </c>
+      <c r="B4">
+        <v>254</v>
+      </c>
+      <c r="C4">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>252</v>
+      </c>
+      <c r="B5">
+        <v>251</v>
+      </c>
+      <c r="C5">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>250</v>
+      </c>
+      <c r="B6">
+        <v>248</v>
+      </c>
+      <c r="C6">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>254</v>
+      </c>
+      <c r="B7">
+        <v>255</v>
+      </c>
+      <c r="C7">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>233</v>
+      </c>
+      <c r="B8">
+        <v>207</v>
+      </c>
+      <c r="C8">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>232</v>
+      </c>
+      <c r="B9">
+        <v>227</v>
+      </c>
+      <c r="C9">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>253</v>
+      </c>
+      <c r="B10">
+        <v>249</v>
+      </c>
+      <c r="C10">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>254</v>
+      </c>
+      <c r="B11">
+        <v>255</v>
+      </c>
+      <c r="C11">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>239</v>
+      </c>
+      <c r="B12">
+        <v>240</v>
+      </c>
+      <c r="C12">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>246</v>
+      </c>
+      <c r="B13">
+        <v>247</v>
+      </c>
+      <c r="C13">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>255</v>
+      </c>
+      <c r="B14">
+        <v>253</v>
+      </c>
+      <c r="C14">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>239</v>
+      </c>
+      <c r="B15">
+        <v>235</v>
+      </c>
+      <c r="C15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>255</v>
+      </c>
+      <c r="B16">
+        <v>255</v>
+      </c>
+      <c r="C16">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>254</v>
+      </c>
+      <c r="B17">
+        <v>254</v>
+      </c>
+      <c r="C17">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>255</v>
+      </c>
+      <c r="B18">
+        <v>241</v>
+      </c>
+      <c r="C18">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>250</v>
+      </c>
+      <c r="B19">
+        <v>249</v>
+      </c>
+      <c r="C19">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>240</v>
+      </c>
+      <c r="B20">
+        <v>235</v>
+      </c>
+      <c r="C20">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>252</v>
+      </c>
+      <c r="B21">
+        <v>248</v>
+      </c>
+      <c r="C21">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>252</v>
+      </c>
+      <c r="B22">
+        <v>173</v>
+      </c>
+      <c r="C22">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>241</v>
+      </c>
+      <c r="B23">
+        <v>217</v>
+      </c>
+      <c r="C23">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>254</v>
+      </c>
+      <c r="B24">
+        <v>252</v>
+      </c>
+      <c r="C24">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>247</v>
+      </c>
+      <c r="B25">
+        <v>247</v>
+      </c>
+      <c r="C25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>251</v>
+      </c>
+      <c r="B26">
+        <v>251</v>
+      </c>
+      <c r="C26">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>254</v>
+      </c>
+      <c r="B27">
+        <v>252</v>
+      </c>
+      <c r="C27">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>253</v>
+      </c>
+      <c r="B28">
+        <v>253</v>
+      </c>
+      <c r="C28">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>255</v>
+      </c>
+      <c r="B29">
+        <v>251</v>
+      </c>
+      <c r="C29">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>252</v>
+      </c>
+      <c r="B30">
+        <v>254</v>
+      </c>
+      <c r="C30">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>251</v>
+      </c>
+      <c r="B31">
+        <v>249</v>
+      </c>
+      <c r="C31">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>247</v>
+      </c>
+      <c r="B32">
+        <v>248</v>
+      </c>
+      <c r="C32">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>253</v>
+      </c>
+      <c r="B33">
+        <v>251</v>
+      </c>
+      <c r="C33">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>254</v>
+      </c>
+      <c r="B34">
+        <v>248</v>
+      </c>
+      <c r="C34">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f>MAX(A2:A34)</f>
+        <v>255</v>
+      </c>
+      <c r="B35">
+        <f>MAX(B2:B34)</f>
+        <v>255</v>
+      </c>
+      <c r="C35">
+        <f>MAX(C2:C34)</f>
+        <v>255</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f>MIN(A2:A34)</f>
+        <v>232</v>
+      </c>
+      <c r="B36">
+        <f>MIN(B2:B34)</f>
+        <v>173</v>
+      </c>
+      <c r="C36">
+        <f>MIN(C2:C34)</f>
+        <v>169</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>